<commit_message>
change all 'na' to 'NA'
</commit_message>
<xml_diff>
--- a/data-raw/Site Metadata Git 4-7-17.xlsx
+++ b/data-raw/Site Metadata Git 4-7-17.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14505"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14510"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -344,9 +344,6 @@
     <t>Armstrong Res. Farm 1</t>
   </si>
   <si>
-    <t>na</t>
-  </si>
-  <si>
     <t>tall cs grass, poplar saplings</t>
   </si>
   <si>
@@ -927,6 +924,9 @@
   </si>
   <si>
     <t>no frost, 1.5" rain before, 1" rain after</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -1408,38 +1408,39 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AV13" sqref="AV13"/>
+      <selection pane="bottomRight" activeCell="AN1" sqref="AN1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" customWidth="1"/>
-    <col min="12" max="13" width="8.5703125" customWidth="1"/>
-    <col min="24" max="26" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.7109375" customWidth="1"/>
-    <col min="28" max="28" width="24.140625" customWidth="1"/>
-    <col min="29" max="30" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16.140625" customWidth="1"/>
-    <col min="35" max="35" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.81640625" customWidth="1"/>
+    <col min="10" max="10" width="9.54296875" customWidth="1"/>
+    <col min="11" max="11" width="9.453125" customWidth="1"/>
+    <col min="12" max="13" width="8.54296875" customWidth="1"/>
+    <col min="24" max="26" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.7265625" customWidth="1"/>
+    <col min="28" max="28" width="24.1796875" customWidth="1"/>
+    <col min="29" max="30" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16.1796875" customWidth="1"/>
+    <col min="35" max="35" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="38.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1579,7 +1580,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>46</v>
       </c>
@@ -1696,7 +1697,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>61</v>
       </c>
@@ -1813,7 +1814,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>64</v>
       </c>
@@ -1863,7 +1864,7 @@
         <v>20</v>
       </c>
       <c r="Q4" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="R4">
         <v>20</v>
@@ -1930,7 +1931,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
         <v>71</v>
       </c>
@@ -1941,7 +1942,7 @@
         <v>73</v>
       </c>
       <c r="D5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E5" s="14">
         <v>100</v>
@@ -2029,7 +2030,7 @@
         <v>87</v>
       </c>
       <c r="AJ5" s="41" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AK5" s="10"/>
       <c r="AL5" s="11"/>
@@ -2041,10 +2042,10 @@
         <v>42822</v>
       </c>
       <c r="AT5" s="33" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
         <v>77</v>
       </c>
@@ -2161,10 +2162,10 @@
         <v>42822</v>
       </c>
       <c r="AT6" s="33" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
-    <row r="7" spans="1:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:46" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="16" t="s">
         <v>80</v>
       </c>
@@ -2196,7 +2197,7 @@
         <v>100</v>
       </c>
       <c r="K7" s="18" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="L7" s="18">
         <v>100</v>
@@ -2205,7 +2206,7 @@
         <v>100</v>
       </c>
       <c r="N7" s="18" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="O7" s="18">
         <v>20</v>
@@ -2214,7 +2215,7 @@
         <v>20</v>
       </c>
       <c r="Q7" s="18" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="R7" s="18">
         <v>20</v>
@@ -2235,7 +2236,7 @@
         <v>84</v>
       </c>
       <c r="X7" s="18" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="Y7" s="24">
         <v>42577</v>
@@ -2288,7 +2289,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
         <v>89</v>
       </c>
@@ -2412,7 +2413,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
         <v>99</v>
       </c>
@@ -2536,7 +2537,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
         <v>103</v>
       </c>
@@ -2568,7 +2569,7 @@
         <v>60</v>
       </c>
       <c r="K10" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="L10">
         <v>60</v>
@@ -2577,7 +2578,7 @@
         <v>60</v>
       </c>
       <c r="N10" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="O10">
         <v>20</v>
@@ -2586,7 +2587,7 @@
         <v>20</v>
       </c>
       <c r="Q10" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="R10">
         <v>20</v>
@@ -2601,13 +2602,13 @@
         <v>300</v>
       </c>
       <c r="V10" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="W10" s="27" t="s">
         <v>94</v>
       </c>
       <c r="X10" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="Y10" s="9">
         <v>42572</v>
@@ -2616,7 +2617,7 @@
         <v>42594</v>
       </c>
       <c r="AB10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AC10" t="s">
         <v>53</v>
@@ -2631,10 +2632,10 @@
         <v>42536</v>
       </c>
       <c r="AH10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AI10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AJ10" s="9">
         <v>42615</v>
@@ -2659,21 +2660,21 @@
         <v>42704</v>
       </c>
       <c r="AT10" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A11" s="13" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="B11" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="C11" t="s">
         <v>111</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>112</v>
-      </c>
-      <c r="D11" t="s">
-        <v>113</v>
       </c>
       <c r="E11" s="14">
         <v>100</v>
@@ -2727,7 +2728,7 @@
         <v>300</v>
       </c>
       <c r="V11" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="W11" s="8" t="s">
         <v>51</v>
@@ -2782,21 +2783,21 @@
         <v>42704</v>
       </c>
       <c r="AT11" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A12" s="13" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="B12" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="C12" t="s">
         <v>116</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>117</v>
-      </c>
-      <c r="D12" t="s">
-        <v>118</v>
       </c>
       <c r="E12" s="14">
         <v>50</v>
@@ -2865,7 +2866,7 @@
         <v>42594</v>
       </c>
       <c r="AB12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AC12" t="s">
         <v>53</v>
@@ -2880,10 +2881,10 @@
         <v>42625</v>
       </c>
       <c r="AH12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AI12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AJ12" s="9">
         <v>42628</v>
@@ -2911,18 +2912,18 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A13" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="C13" t="s">
         <v>121</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>122</v>
-      </c>
-      <c r="D13" t="s">
-        <v>123</v>
       </c>
       <c r="E13" s="14">
         <v>50</v>
@@ -2943,7 +2944,7 @@
         <v>50</v>
       </c>
       <c r="K13" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="L13">
         <v>50</v>
@@ -2952,7 +2953,7 @@
         <v>50</v>
       </c>
       <c r="N13" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="O13">
         <v>20</v>
@@ -2961,7 +2962,7 @@
         <v>20</v>
       </c>
       <c r="Q13" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="R13">
         <v>6</v>
@@ -2982,7 +2983,7 @@
         <v>94</v>
       </c>
       <c r="X13" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="Y13" s="9">
         <v>42571</v>
@@ -3037,18 +3038,18 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A14" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="C14" t="s">
         <v>125</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>126</v>
-      </c>
-      <c r="D14" t="s">
-        <v>127</v>
       </c>
       <c r="E14" s="14">
         <v>100</v>
@@ -3158,18 +3159,18 @@
         <v>42711</v>
       </c>
       <c r="AT14" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A15" s="13" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="B15" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="C15" t="s">
         <v>130</v>
-      </c>
-      <c r="C15" t="s">
-        <v>131</v>
       </c>
       <c r="D15" t="s">
         <v>83</v>
@@ -3226,7 +3227,7 @@
         <v>30</v>
       </c>
       <c r="V15" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="W15" s="8" t="s">
         <v>51</v>
@@ -3244,13 +3245,13 @@
         <v>42599</v>
       </c>
       <c r="AB15" t="s">
+        <v>131</v>
+      </c>
+      <c r="AC15" t="s">
         <v>132</v>
       </c>
-      <c r="AC15" t="s">
-        <v>133</v>
-      </c>
       <c r="AD15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AE15" t="s">
         <v>95</v>
@@ -3287,18 +3288,18 @@
         <v>42705</v>
       </c>
       <c r="AT15" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="C16" t="s">
         <v>135</v>
-      </c>
-      <c r="C16" t="s">
-        <v>136</v>
       </c>
       <c r="D16" t="s">
         <v>83</v>
@@ -3322,7 +3323,7 @@
         <v>100</v>
       </c>
       <c r="K16" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="L16">
         <v>100</v>
@@ -3331,7 +3332,7 @@
         <v>100</v>
       </c>
       <c r="N16" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="O16">
         <v>20</v>
@@ -3340,10 +3341,10 @@
         <v>20</v>
       </c>
       <c r="Q16" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="R16" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="S16">
         <v>22</v>
@@ -3355,13 +3356,13 @@
         <v>10</v>
       </c>
       <c r="V16" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="W16" s="8" t="s">
         <v>51</v>
       </c>
       <c r="X16" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="Y16" s="9">
         <v>42571</v>
@@ -3370,13 +3371,13 @@
         <v>42592</v>
       </c>
       <c r="AB16" t="s">
+        <v>131</v>
+      </c>
+      <c r="AC16" t="s">
         <v>132</v>
       </c>
-      <c r="AC16" t="s">
-        <v>133</v>
-      </c>
       <c r="AD16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AE16" t="s">
         <v>95</v>
@@ -3413,21 +3414,21 @@
         <v>42705</v>
       </c>
       <c r="AT16" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B17" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="C17" t="s">
         <v>138</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>139</v>
-      </c>
-      <c r="D17" t="s">
-        <v>140</v>
       </c>
       <c r="E17" s="26">
         <v>75</v>
@@ -3442,7 +3443,7 @@
         <v>1.1119725</v>
       </c>
       <c r="I17" s="26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J17">
         <v>80</v>
@@ -3496,13 +3497,13 @@
         <v>42594</v>
       </c>
       <c r="AB17" t="s">
+        <v>141</v>
+      </c>
+      <c r="AC17" t="s">
         <v>142</v>
       </c>
-      <c r="AC17" t="s">
-        <v>143</v>
-      </c>
       <c r="AD17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AE17" t="s">
         <v>95</v>
@@ -3519,10 +3520,10 @@
       <c r="AK17" s="10"/>
       <c r="AL17" s="11"/>
       <c r="AM17" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="AN17" s="14" t="s">
         <v>144</v>
-      </c>
-      <c r="AN17" s="14" t="s">
-        <v>145</v>
       </c>
       <c r="AO17" s="12"/>
       <c r="AP17" s="12"/>
@@ -3530,21 +3531,21 @@
         <v>42707</v>
       </c>
       <c r="AT17" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="B18" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="C18" t="s">
         <v>147</v>
       </c>
-      <c r="C18" t="s">
-        <v>148</v>
-      </c>
       <c r="D18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E18" s="26">
         <v>75</v>
@@ -3559,7 +3560,7 @@
         <v>1.1119725</v>
       </c>
       <c r="I18" s="26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J18">
         <v>80</v>
@@ -3625,10 +3626,10 @@
         <v>95</v>
       </c>
       <c r="AH18" t="s">
+        <v>148</v>
+      </c>
+      <c r="AI18" t="s">
         <v>149</v>
-      </c>
-      <c r="AI18" t="s">
-        <v>150</v>
       </c>
       <c r="AJ18" s="9">
         <v>42621</v>
@@ -3653,27 +3654,27 @@
         <v>42707</v>
       </c>
       <c r="AT18" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
-    <row r="19" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A19" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B19" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="C19" t="s">
         <v>152</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>153</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="F19" s="7" t="s">
         <v>155</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>156</v>
       </c>
       <c r="G19">
         <v>860</v>
@@ -3682,7 +3683,7 @@
         <v>0.21251030000000001</v>
       </c>
       <c r="I19" s="26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J19">
         <v>60</v>
@@ -3706,7 +3707,7 @@
         <v>20</v>
       </c>
       <c r="Q19" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="R19">
         <v>7</v>
@@ -3736,7 +3737,7 @@
         <v>42594</v>
       </c>
       <c r="AB19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AC19" t="s">
         <v>53</v>
@@ -3779,27 +3780,27 @@
         <v>42705</v>
       </c>
       <c r="AT19" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A20" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="B20" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="C20" t="s">
         <v>159</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>160</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="F20" s="7" t="s">
         <v>162</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>163</v>
       </c>
       <c r="G20">
         <v>860</v>
@@ -3808,7 +3809,7 @@
         <v>0.21251030000000001</v>
       </c>
       <c r="I20" s="26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J20">
         <v>60</v>
@@ -3832,7 +3833,7 @@
         <v>20</v>
       </c>
       <c r="Q20" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="R20">
         <v>7</v>
@@ -3862,7 +3863,7 @@
         <v>42594</v>
       </c>
       <c r="AB20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AC20" t="s">
         <v>53</v>
@@ -3905,18 +3906,18 @@
         <v>42705</v>
       </c>
       <c r="AT20" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="B21" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="C21" t="s">
         <v>166</v>
-      </c>
-      <c r="C21" t="s">
-        <v>167</v>
       </c>
       <c r="D21" t="s">
         <v>83</v>
@@ -3973,7 +3974,7 @@
         <v>60</v>
       </c>
       <c r="V21" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="W21" s="27" t="s">
         <v>94</v>
@@ -4000,10 +4001,10 @@
         <v>95</v>
       </c>
       <c r="AH21" t="s">
+        <v>148</v>
+      </c>
+      <c r="AI21" t="s">
         <v>149</v>
-      </c>
-      <c r="AI21" t="s">
-        <v>150</v>
       </c>
       <c r="AJ21" s="9">
         <v>42615</v>
@@ -4028,18 +4029,18 @@
         <v>42704</v>
       </c>
       <c r="AT21" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="B22" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="C22" t="s">
         <v>169</v>
-      </c>
-      <c r="C22" t="s">
-        <v>170</v>
       </c>
       <c r="D22" t="s">
         <v>83</v>
@@ -4096,7 +4097,7 @@
         <v>60</v>
       </c>
       <c r="V22" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="W22" s="8" t="s">
         <v>51</v>
@@ -4123,10 +4124,10 @@
         <v>95</v>
       </c>
       <c r="AH22" t="s">
+        <v>148</v>
+      </c>
+      <c r="AI22" t="s">
         <v>149</v>
-      </c>
-      <c r="AI22" t="s">
-        <v>150</v>
       </c>
       <c r="AJ22" s="9">
         <v>42615</v>
@@ -4151,21 +4152,21 @@
         <v>42704</v>
       </c>
       <c r="AT22" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="B23" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="C23" t="s">
         <v>172</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>173</v>
-      </c>
-      <c r="D23" t="s">
-        <v>174</v>
       </c>
       <c r="E23">
         <v>50</v>
@@ -4186,28 +4187,28 @@
         <v>50</v>
       </c>
       <c r="K23" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="L23" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="M23">
         <v>50</v>
       </c>
       <c r="N23" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="O23" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="P23">
         <v>20</v>
       </c>
       <c r="Q23" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="R23" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="S23">
         <v>20</v>
@@ -4225,10 +4226,10 @@
         <v>51</v>
       </c>
       <c r="X23" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="Y23" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="Z23" s="9">
         <v>42597</v>
@@ -4249,10 +4250,10 @@
         <v>42628</v>
       </c>
       <c r="AH23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AI23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AJ23" s="9">
         <v>42648</v>
@@ -4277,21 +4278,21 @@
         <v>42710</v>
       </c>
       <c r="AT23" s="9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="24" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A24" s="13" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="24" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
+      <c r="B24" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="C24" t="s">
         <v>178</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>179</v>
-      </c>
-      <c r="D24" t="s">
-        <v>180</v>
       </c>
       <c r="E24">
         <v>103</v>
@@ -4360,22 +4361,22 @@
         <v>42593</v>
       </c>
       <c r="AB24" t="s">
+        <v>180</v>
+      </c>
+      <c r="AC24" t="s">
         <v>181</v>
       </c>
-      <c r="AC24" t="s">
-        <v>182</v>
-      </c>
       <c r="AD24" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AE24" t="s">
         <v>95</v>
       </c>
       <c r="AH24" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AI24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AJ24" s="12"/>
       <c r="AK24" s="12"/>
@@ -4393,18 +4394,18 @@
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:64" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:64" s="37" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="B25" s="36" t="s">
         <v>293</v>
       </c>
-      <c r="B25" s="36" t="s">
+      <c r="C25" s="37" t="s">
         <v>294</v>
       </c>
-      <c r="C25" s="37" t="s">
+      <c r="D25" s="37" t="s">
         <v>295</v>
-      </c>
-      <c r="D25" s="37" t="s">
-        <v>296</v>
       </c>
       <c r="E25" s="37">
         <v>25</v>
@@ -4420,7 +4421,7 @@
         <v>0.13096565000000002</v>
       </c>
       <c r="I25" s="38" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J25" s="37">
         <v>30</v>
@@ -4466,7 +4467,7 @@
       </c>
       <c r="AA25" s="39"/>
       <c r="AB25" s="37" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="AC25" s="37" t="s">
         <v>53</v>
@@ -4512,15 +4513,15 @@
       <c r="BK25" s="40"/>
       <c r="BL25" s="40"/>
     </row>
-    <row r="26" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="B26" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="C26" t="s">
         <v>185</v>
-      </c>
-      <c r="C26" t="s">
-        <v>186</v>
       </c>
       <c r="D26" t="s">
         <v>83</v>
@@ -4592,7 +4593,7 @@
         <v>42593</v>
       </c>
       <c r="AB26" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AC26" t="s">
         <v>53</v>
@@ -4635,18 +4636,18 @@
         <v>42712</v>
       </c>
       <c r="AT26" s="9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="27" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A27" s="13" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="27" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
+      <c r="B27" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="C27" t="s">
         <v>190</v>
-      </c>
-      <c r="C27" t="s">
-        <v>191</v>
       </c>
       <c r="D27" t="s">
         <v>83</v>
@@ -4761,21 +4762,21 @@
         <v>42712</v>
       </c>
       <c r="AT27" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
-    <row r="28" spans="1:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="B28" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="C28" s="18" t="s">
         <v>193</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="D28" s="18" t="s">
         <v>194</v>
-      </c>
-      <c r="D28" s="18" t="s">
-        <v>195</v>
       </c>
       <c r="E28" s="18">
         <v>106</v>
@@ -4829,7 +4830,7 @@
         <v>5</v>
       </c>
       <c r="V28" s="18" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="W28" s="30" t="s">
         <v>51</v>
@@ -4845,7 +4846,7 @@
       </c>
       <c r="AA28" s="18"/>
       <c r="AB28" s="18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AC28" s="18" t="s">
         <v>53</v>
@@ -4861,10 +4862,10 @@
         <v>42614</v>
       </c>
       <c r="AH28" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AI28" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AJ28" s="24">
         <v>42627</v>
@@ -4891,21 +4892,21 @@
         <v>42711</v>
       </c>
       <c r="AT28" s="24" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="29" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A29" s="13" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="29" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
+      <c r="B29" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="C29" t="s">
         <v>199</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" s="15" t="s">
         <v>200</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>201</v>
       </c>
       <c r="E29" s="14">
         <v>35</v>
@@ -4986,7 +4987,7 @@
         <v>54</v>
       </c>
       <c r="AE29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AH29" t="s">
         <v>96</v>
@@ -5013,21 +5014,21 @@
         <v>42713</v>
       </c>
       <c r="AT29" s="33" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="30" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A30" s="13" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="30" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
+      <c r="B30" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="C30" t="s">
         <v>205</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>206</v>
-      </c>
-      <c r="D30" t="s">
-        <v>207</v>
       </c>
       <c r="E30" s="14">
         <v>54</v>
@@ -5096,7 +5097,7 @@
         <v>42593</v>
       </c>
       <c r="AB30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AC30" t="s">
         <v>53</v>
@@ -5105,16 +5106,16 @@
         <v>53</v>
       </c>
       <c r="AE30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AG30" s="9">
         <v>42619</v>
       </c>
       <c r="AH30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AI30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AJ30" s="9">
         <v>42641</v>
@@ -5132,10 +5133,10 @@
         <v>59</v>
       </c>
       <c r="AO30" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AP30" s="14" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="AQ30" s="14" t="s">
         <v>58</v>
@@ -5147,21 +5148,21 @@
         <v>42710</v>
       </c>
       <c r="AT30" s="34" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="31" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A31" s="13" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="31" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
+      <c r="B31" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="C31" t="s">
         <v>212</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>213</v>
-      </c>
-      <c r="D31" t="s">
-        <v>214</v>
       </c>
       <c r="E31" s="14">
         <v>50</v>
@@ -5233,13 +5234,13 @@
         <v>85</v>
       </c>
       <c r="AC31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AD31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AE31" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AH31" t="s">
         <v>87</v>
@@ -5255,10 +5256,10 @@
       </c>
       <c r="AL31" s="11"/>
       <c r="AM31" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="AN31" s="14" t="s">
         <v>144</v>
-      </c>
-      <c r="AN31" s="14" t="s">
-        <v>145</v>
       </c>
       <c r="AO31" s="14" t="s">
         <v>58</v>
@@ -5273,18 +5274,18 @@
         <v>98</v>
       </c>
     </row>
-    <row r="32" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A32" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="B32" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="C32" t="s">
         <v>217</v>
       </c>
-      <c r="C32" t="s">
-        <v>218</v>
-      </c>
       <c r="D32" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E32" s="14">
         <v>50</v>
@@ -5299,7 +5300,7 @@
         <v>0.18532875000000001</v>
       </c>
       <c r="I32" s="26" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J32">
         <v>50</v>
@@ -5365,16 +5366,16 @@
         <v>53</v>
       </c>
       <c r="AE32" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AG32" s="9">
         <v>42614</v>
       </c>
       <c r="AH32" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AI32" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AJ32" s="9">
         <v>42622</v>
@@ -5402,18 +5403,18 @@
         <v>98</v>
       </c>
     </row>
-    <row r="33" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A33" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="B33" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="C33" t="s">
         <v>221</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>222</v>
-      </c>
-      <c r="D33" t="s">
-        <v>223</v>
       </c>
       <c r="E33" s="14">
         <v>50</v>
@@ -5485,7 +5486,7 @@
         <v>42599</v>
       </c>
       <c r="AB33" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AC33" t="s">
         <v>53</v>
@@ -5494,16 +5495,16 @@
         <v>53</v>
       </c>
       <c r="AE33" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AG33" s="9">
         <v>42639</v>
       </c>
       <c r="AH33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AI33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AJ33" s="11">
         <v>42662</v>
@@ -5528,21 +5529,21 @@
         <v>42710</v>
       </c>
       <c r="AT33" s="9" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="34" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A34" s="13" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="34" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
+      <c r="B34" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="C34" t="s">
         <v>227</v>
       </c>
-      <c r="C34" t="s">
-        <v>228</v>
-      </c>
       <c r="D34" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E34" s="14">
         <v>50</v>
@@ -5596,7 +5597,7 @@
         <v>350</v>
       </c>
       <c r="V34" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="W34" s="8" t="s">
         <v>51</v>
@@ -5614,7 +5615,7 @@
         <v>42599</v>
       </c>
       <c r="AB34" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AC34" t="s">
         <v>53</v>
@@ -5623,7 +5624,7 @@
         <v>53</v>
       </c>
       <c r="AE34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AH34" t="s">
         <v>96</v>
@@ -5654,21 +5655,21 @@
         <v>42710</v>
       </c>
       <c r="AT34" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
-    <row r="35" spans="1:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:46" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="B35" s="17" t="s">
         <v>229</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="C35" s="18" t="s">
         <v>230</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="D35" s="18" t="s">
         <v>231</v>
-      </c>
-      <c r="D35" s="18" t="s">
-        <v>232</v>
       </c>
       <c r="E35" s="18">
         <v>50</v>
@@ -5722,7 +5723,7 @@
         <v>10</v>
       </c>
       <c r="V35" s="18" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="W35" s="22" t="s">
         <v>84</v>
@@ -5740,16 +5741,16 @@
         <v>42599</v>
       </c>
       <c r="AB35" s="18" t="s">
+        <v>232</v>
+      </c>
+      <c r="AC35" s="18" t="s">
         <v>233</v>
       </c>
-      <c r="AC35" s="18" t="s">
-        <v>234</v>
-      </c>
       <c r="AD35" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AE35" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AF35" s="18"/>
       <c r="AG35" s="18"/>
@@ -5778,21 +5779,21 @@
         <v>42710</v>
       </c>
       <c r="AT35" s="24" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="36" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A36" s="13" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="36" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
+      <c r="B36" s="14" t="s">
         <v>236</v>
       </c>
-      <c r="B36" s="14" t="s">
+      <c r="C36" t="s">
         <v>237</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>238</v>
-      </c>
-      <c r="D36" t="s">
-        <v>239</v>
       </c>
       <c r="E36" s="14">
         <v>83</v>
@@ -5831,7 +5832,7 @@
         <v>20</v>
       </c>
       <c r="Q36" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="R36" s="14">
         <v>20</v>
@@ -5871,13 +5872,13 @@
         <v>53</v>
       </c>
       <c r="AE36" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AH36" t="s">
         <v>56</v>
       </c>
       <c r="AI36" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AJ36" s="9">
         <v>42614</v>
@@ -5896,24 +5897,24 @@
         <v>58</v>
       </c>
       <c r="AP36" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AS36" s="9">
         <v>42706</v>
       </c>
       <c r="AT36" s="9" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="37" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A37" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="B37" s="14" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="37" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="s">
-        <v>236</v>
-      </c>
-      <c r="B37" s="14" t="s">
+      <c r="C37" t="s">
         <v>244</v>
-      </c>
-      <c r="C37" t="s">
-        <v>245</v>
       </c>
       <c r="D37" t="s">
         <v>83</v>
@@ -5955,7 +5956,7 @@
         <v>20</v>
       </c>
       <c r="Q37" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="R37" s="14">
         <v>20</v>
@@ -5995,13 +5996,13 @@
         <v>53</v>
       </c>
       <c r="AE37" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AH37" t="s">
         <v>56</v>
       </c>
       <c r="AI37" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AJ37" s="9">
         <v>42614</v>
@@ -6020,27 +6021,27 @@
         <v>58</v>
       </c>
       <c r="AP37" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AS37" s="9">
         <v>42706</v>
       </c>
       <c r="AT37" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
-    <row r="38" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A38" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="B38" s="14" t="s">
         <v>246</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="C38" t="s">
         <v>247</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>248</v>
-      </c>
-      <c r="D38" t="s">
-        <v>249</v>
       </c>
       <c r="E38" s="14">
         <v>100</v>
@@ -6079,7 +6080,7 @@
         <v>20</v>
       </c>
       <c r="Q38" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="R38" s="14">
         <v>20</v>
@@ -6119,13 +6120,13 @@
         <v>53</v>
       </c>
       <c r="AE38" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AH38" t="s">
         <v>56</v>
       </c>
       <c r="AI38" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AJ38" s="9">
         <v>42614</v>
@@ -6144,33 +6145,33 @@
         <v>58</v>
       </c>
       <c r="AP38" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AS38" s="9">
         <v>42706</v>
       </c>
       <c r="AT38" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
-    <row r="39" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A39" s="13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B39" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="C39" t="s">
         <v>250</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>251</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="E39" s="7" t="s">
-        <v>253</v>
-      </c>
       <c r="F39" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G39">
         <v>1900</v>
@@ -6179,7 +6180,7 @@
         <v>0.46949950000000001</v>
       </c>
       <c r="I39" s="26" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J39">
         <v>50</v>
@@ -6203,7 +6204,7 @@
         <v>20</v>
       </c>
       <c r="Q39" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="R39" s="14">
         <v>20</v>
@@ -6242,13 +6243,13 @@
         <v>53</v>
       </c>
       <c r="AE39" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AH39" t="s">
         <v>56</v>
       </c>
       <c r="AI39" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AJ39" s="9">
         <v>42614</v>
@@ -6267,27 +6268,27 @@
         <v>58</v>
       </c>
       <c r="AP39" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AS39" s="9">
         <v>42706</v>
       </c>
       <c r="AT39" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
-    <row r="40" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A40" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="B40" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="C40" t="s">
         <v>256</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>257</v>
-      </c>
-      <c r="D40" t="s">
-        <v>258</v>
       </c>
       <c r="E40" s="7">
         <v>108</v>
@@ -6366,13 +6367,13 @@
         <v>53</v>
       </c>
       <c r="AE40" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AH40" t="s">
         <v>56</v>
       </c>
       <c r="AI40" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AJ40" s="9">
         <v>42614</v>
@@ -6391,33 +6392,33 @@
         <v>58</v>
       </c>
       <c r="AP40" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AS40" s="9">
         <v>42706</v>
       </c>
       <c r="AT40" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
-    <row r="41" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A41" s="13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B41" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="C41" t="s">
         <v>259</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>260</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="E41" s="7" t="s">
-        <v>262</v>
-      </c>
       <c r="F41" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G41">
         <v>450</v>
@@ -6426,7 +6427,7 @@
         <v>0.11119725000000001</v>
       </c>
       <c r="I41" s="26" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J41" s="7">
         <v>50</v>
@@ -6489,13 +6490,13 @@
         <v>53</v>
       </c>
       <c r="AE41" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AH41" t="s">
         <v>56</v>
       </c>
       <c r="AI41" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AJ41" s="9">
         <v>42614</v>
@@ -6514,27 +6515,27 @@
         <v>58</v>
       </c>
       <c r="AP41" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AS41" s="9">
         <v>42706</v>
       </c>
       <c r="AT41" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
-    <row r="42" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A42" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="B42" s="14" t="s">
         <v>264</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="C42" t="s">
         <v>265</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>266</v>
-      </c>
-      <c r="D42" t="s">
-        <v>267</v>
       </c>
       <c r="E42" s="7">
         <v>90</v>
@@ -6573,7 +6574,7 @@
         <v>20</v>
       </c>
       <c r="Q42" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="R42">
         <v>20</v>
@@ -6612,13 +6613,13 @@
         <v>53</v>
       </c>
       <c r="AE42" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AH42" t="s">
         <v>56</v>
       </c>
       <c r="AI42" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AJ42" s="9">
         <v>42614</v>
@@ -6637,24 +6638,24 @@
         <v>58</v>
       </c>
       <c r="AP42" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AS42" s="9">
         <v>42706</v>
       </c>
       <c r="AT42" s="9" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="43" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A43" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="B43" s="14" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="43" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="s">
-        <v>264</v>
-      </c>
-      <c r="B43" s="14" t="s">
+      <c r="C43" t="s">
         <v>269</v>
-      </c>
-      <c r="C43" t="s">
-        <v>270</v>
       </c>
       <c r="D43" t="s">
         <v>49</v>
@@ -6732,16 +6733,16 @@
         <v>53</v>
       </c>
       <c r="AD43" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AE43" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AH43" t="s">
         <v>56</v>
       </c>
       <c r="AI43" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AJ43" s="9">
         <v>42614</v>
@@ -6760,27 +6761,27 @@
         <v>58</v>
       </c>
       <c r="AP43" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AS43" s="9">
         <v>42706</v>
       </c>
       <c r="AT43" s="9" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="44" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A44" s="13" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="44" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A44" s="13" t="s">
+      <c r="B44" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B44" s="14" t="s">
+      <c r="C44" t="s">
         <v>274</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>275</v>
-      </c>
-      <c r="D44" t="s">
-        <v>276</v>
       </c>
       <c r="E44">
         <v>55</v>
@@ -6801,7 +6802,7 @@
         <v>50</v>
       </c>
       <c r="K44" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="L44">
         <v>50</v>
@@ -6810,7 +6811,7 @@
         <v>50</v>
       </c>
       <c r="N44" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="O44">
         <v>10</v>
@@ -6819,7 +6820,7 @@
         <v>20</v>
       </c>
       <c r="Q44" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="R44">
         <v>10</v>
@@ -6840,7 +6841,7 @@
         <v>51</v>
       </c>
       <c r="X44" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="Y44" s="31">
         <v>42565</v>
@@ -6858,13 +6859,13 @@
         <v>53</v>
       </c>
       <c r="AE44" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AH44" t="s">
         <v>56</v>
       </c>
       <c r="AI44" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AJ44" s="9">
         <v>42614</v>
@@ -6883,27 +6884,27 @@
         <v>58</v>
       </c>
       <c r="AP44" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AS44" s="9">
         <v>42713</v>
       </c>
       <c r="AT44" s="9" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="45" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A45" s="13" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="45" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="s">
+      <c r="B45" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="B45" s="14" t="s">
+      <c r="C45" t="s">
         <v>279</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>280</v>
-      </c>
-      <c r="D45" t="s">
-        <v>281</v>
       </c>
       <c r="E45">
         <v>55</v>
@@ -6924,7 +6925,7 @@
         <v>50</v>
       </c>
       <c r="K45" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="L45">
         <v>50</v>
@@ -6933,7 +6934,7 @@
         <v>50</v>
       </c>
       <c r="N45" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="O45">
         <v>10</v>
@@ -6942,7 +6943,7 @@
         <v>20</v>
       </c>
       <c r="Q45" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="R45">
         <v>10</v>
@@ -6963,7 +6964,7 @@
         <v>51</v>
       </c>
       <c r="X45" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="Y45" s="31">
         <v>42565</v>
@@ -6981,13 +6982,13 @@
         <v>53</v>
       </c>
       <c r="AE45" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AH45" t="s">
         <v>56</v>
       </c>
       <c r="AI45" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AJ45" s="9">
         <v>42614</v>
@@ -7006,27 +7007,27 @@
         <v>58</v>
       </c>
       <c r="AP45" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AS45" s="9">
         <v>42713</v>
       </c>
       <c r="AT45" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
-    <row r="46" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A46" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="B46" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="B46" s="14" t="s">
+      <c r="C46" t="s">
         <v>283</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>284</v>
-      </c>
-      <c r="D46" t="s">
-        <v>285</v>
       </c>
       <c r="E46">
         <v>30</v>
@@ -7047,7 +7048,7 @@
         <v>30</v>
       </c>
       <c r="K46" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="L46">
         <v>30</v>
@@ -7056,7 +7057,7 @@
         <v>30</v>
       </c>
       <c r="N46" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="O46">
         <v>20</v>
@@ -7065,13 +7066,13 @@
         <v>20</v>
       </c>
       <c r="Q46" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="R46">
         <v>10</v>
       </c>
       <c r="S46" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="T46">
         <v>79</v>
@@ -7086,7 +7087,7 @@
         <v>51</v>
       </c>
       <c r="X46" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="Y46" s="31">
         <v>42570</v>
@@ -7104,13 +7105,13 @@
         <v>53</v>
       </c>
       <c r="AE46" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AH46" t="s">
         <v>56</v>
       </c>
       <c r="AI46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AJ46" s="9">
         <v>42627</v>
@@ -7135,21 +7136,21 @@
         <v>42705</v>
       </c>
       <c r="AT46" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
-    <row r="47" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A47" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="B47" s="14" t="s">
         <v>286</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="C47" t="s">
         <v>287</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>288</v>
-      </c>
-      <c r="D47" t="s">
-        <v>289</v>
       </c>
       <c r="E47">
         <v>54</v>
@@ -7170,28 +7171,28 @@
         <v>50</v>
       </c>
       <c r="K47" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="L47" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="M47">
         <v>50</v>
       </c>
       <c r="N47" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="O47" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="P47">
         <v>20</v>
       </c>
       <c r="Q47" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="R47" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="S47">
         <v>20</v>
@@ -7209,16 +7210,16 @@
         <v>51</v>
       </c>
       <c r="X47" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="Y47" t="s">
-        <v>106</v>
+        <v>300</v>
       </c>
       <c r="Z47" s="31">
         <v>42597</v>
       </c>
       <c r="AB47" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AC47" t="s">
         <v>53</v>
@@ -7227,13 +7228,13 @@
         <v>53</v>
       </c>
       <c r="AE47" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AH47" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AI47" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AJ47" s="9">
         <v>42627</v>
@@ -7258,7 +7259,7 @@
         <v>42713</v>
       </c>
       <c r="AT47" s="33" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update metadata columns. Change column titles from 'r1_transect_length' style to '2016_r1_transect_length' style. Change blanks in transect_length columns to 'NA' and turn cells gray. Add yellow color to transects that changed length.
</commit_message>
<xml_diff>
--- a/data-raw/Site Metadata Git 4-7-17.xlsx
+++ b/data-raw/Site Metadata Git 4-7-17.xlsx
@@ -15,7 +15,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="301">
   <si>
     <t>site_id</t>
   </si>
@@ -57,15 +57,6 @@
     <t>final_transect_length</t>
   </si>
   <si>
-    <t>r1_transect_length</t>
-  </si>
-  <si>
-    <t>r2_transect_length</t>
-  </si>
-  <si>
-    <t>r3_transect_length</t>
-  </si>
-  <si>
     <t>r1_section_length</t>
   </si>
   <si>
@@ -925,6 +916,18 @@
   </si>
   <si>
     <t>70*30</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>2016_r1_transect_length</t>
+  </si>
+  <si>
+    <t>2016_r2_transect_length</t>
+  </si>
+  <si>
+    <t>2016_r3_transect_length</t>
   </si>
 </sst>
 </file>
@@ -954,7 +957,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -989,6 +992,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDBDBDB"/>
         <bgColor rgb="FFDEEBF7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1063,7 +1078,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1119,6 +1134,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1473,7 +1493,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H50" sqref="H50"/>
+      <selection pane="bottomRight" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1542,126 +1562,126 @@
         <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="2" t="s">
+      <c r="X1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AF1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AG1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AH1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AS1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AT1" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="AR1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AS1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AT1" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" t="s">
         <v>46</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" t="s">
-        <v>49</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -1676,7 +1696,7 @@
         <v>0.24710499999999999</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J2">
         <v>100</v>
@@ -1718,7 +1738,7 @@
         <v>50</v>
       </c>
       <c r="W2" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X2" s="9">
         <v>42549</v>
@@ -1730,22 +1750,22 @@
         <v>42597</v>
       </c>
       <c r="AB2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE2" t="s">
         <v>52</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AH2" t="s">
         <v>53</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AI2" t="s">
         <v>54</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>57</v>
       </c>
       <c r="AJ2" s="9">
         <v>42675</v>
@@ -1753,10 +1773,10 @@
       <c r="AK2" s="10"/>
       <c r="AL2" s="11"/>
       <c r="AM2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO2" s="12"/>
       <c r="AP2" s="12"/>
@@ -1764,21 +1784,21 @@
         <v>42695</v>
       </c>
       <c r="AT2" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E3">
         <v>100</v>
@@ -1793,7 +1813,7 @@
         <v>0.24710499999999999</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J3">
         <v>100</v>
@@ -1835,7 +1855,7 @@
         <v>50</v>
       </c>
       <c r="W3" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X3" s="9">
         <v>42549</v>
@@ -1847,22 +1867,22 @@
         <v>42597</v>
       </c>
       <c r="AB3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE3" t="s">
         <v>52</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AH3" t="s">
         <v>53</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AI3" t="s">
         <v>54</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>57</v>
       </c>
       <c r="AJ3" s="9">
         <v>42675</v>
@@ -1870,10 +1890,10 @@
       <c r="AK3" s="10"/>
       <c r="AL3" s="11"/>
       <c r="AM3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO3" s="12"/>
       <c r="AP3" s="12"/>
@@ -1881,21 +1901,21 @@
         <v>42695</v>
       </c>
       <c r="AT3" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" t="s">
         <v>64</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" t="s">
-        <v>67</v>
       </c>
       <c r="E4">
         <v>77</v>
@@ -1910,7 +1930,7 @@
         <v>0.15221667999999999</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J4">
         <v>70</v>
@@ -1949,7 +1969,7 @@
         <v>30</v>
       </c>
       <c r="W4" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X4" s="9">
         <v>42551</v>
@@ -1961,22 +1981,22 @@
         <v>42595</v>
       </c>
       <c r="AB4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH4" t="s">
         <v>53</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AI4" t="s">
         <v>54</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>57</v>
       </c>
       <c r="AJ4" s="9">
         <v>42628</v>
@@ -1984,10 +2004,10 @@
       <c r="AK4" s="12"/>
       <c r="AL4" s="15"/>
       <c r="AM4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO4" s="12"/>
       <c r="AP4" s="12"/>
@@ -1995,21 +2015,21 @@
         <v>42696</v>
       </c>
       <c r="AT4" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" t="s">
         <v>71</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" t="s">
-        <v>74</v>
       </c>
       <c r="E5" s="14">
         <v>100</v>
@@ -2024,7 +2044,7 @@
         <v>0.12</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J5">
         <v>100</v>
@@ -2066,7 +2086,7 @@
         <v>400</v>
       </c>
       <c r="W5" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X5" s="9">
         <v>42549</v>
@@ -2078,26 +2098,26 @@
         <v>42597</v>
       </c>
       <c r="AB5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="AC5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AD5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="AE5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="AG5" s="9"/>
       <c r="AH5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="AI5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="AJ5" s="16" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="AK5" s="10"/>
       <c r="AL5" s="11"/>
@@ -2109,21 +2129,21 @@
         <v>42822</v>
       </c>
       <c r="AT5" s="17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" t="s">
         <v>79</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D6" t="s">
-        <v>82</v>
       </c>
       <c r="E6" s="14">
         <v>100</v>
@@ -2138,7 +2158,7 @@
         <v>0.14826300000000001</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J6">
         <v>100</v>
@@ -2180,7 +2200,7 @@
         <v>400</v>
       </c>
       <c r="W6" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X6" s="9">
         <v>42549</v>
@@ -2192,25 +2212,25 @@
         <v>42597</v>
       </c>
       <c r="AB6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="AC6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AD6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="AE6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="AG6" s="9">
         <v>42667</v>
       </c>
       <c r="AH6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AI6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AJ6" s="9">
         <v>42675</v>
@@ -2218,10 +2238,10 @@
       <c r="AK6" s="10"/>
       <c r="AL6" s="11"/>
       <c r="AM6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO6" s="12"/>
       <c r="AP6" s="12"/>
@@ -2229,21 +2249,21 @@
         <v>42822</v>
       </c>
       <c r="AT6" s="17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="20" t="s">
         <v>84</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>87</v>
       </c>
       <c r="E7" s="20">
         <v>100</v>
@@ -2258,12 +2278,14 @@
         <v>0.49420999999999998</v>
       </c>
       <c r="I7" s="22" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J7" s="20">
         <v>100</v>
       </c>
-      <c r="K7" s="20"/>
+      <c r="K7" s="41" t="s">
+        <v>297</v>
+      </c>
       <c r="L7" s="20">
         <v>100</v>
       </c>
@@ -2294,7 +2316,7 @@
         <v>10</v>
       </c>
       <c r="W7" s="23" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="X7" s="20"/>
       <c r="Y7" s="24">
@@ -2305,26 +2327,26 @@
       </c>
       <c r="AA7" s="20"/>
       <c r="AB7" s="20" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="AC7" s="20" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="AD7" s="20" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="AE7" s="20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="AF7" s="24">
         <v>42683</v>
       </c>
       <c r="AG7" s="20"/>
       <c r="AH7" s="20" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="AI7" s="20" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="AJ7" s="24">
         <v>42661</v>
@@ -2332,10 +2354,10 @@
       <c r="AK7" s="25"/>
       <c r="AL7" s="26"/>
       <c r="AM7" s="20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN7" s="20" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO7" s="27"/>
       <c r="AP7" s="27"/>
@@ -2345,21 +2367,21 @@
         <v>42695</v>
       </c>
       <c r="AT7" s="24" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" t="s">
         <v>92</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="C8" t="s">
-        <v>94</v>
-      </c>
-      <c r="D8" t="s">
-        <v>95</v>
       </c>
       <c r="E8" s="14">
         <v>54</v>
@@ -2374,7 +2396,7 @@
         <v>0.37016328999999998</v>
       </c>
       <c r="I8" s="28" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J8">
         <v>50</v>
@@ -2416,7 +2438,7 @@
         <v>40</v>
       </c>
       <c r="W8" s="29" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="X8" s="9">
         <v>42551</v>
@@ -2429,22 +2451,22 @@
       </c>
       <c r="AA8" s="14"/>
       <c r="AB8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="AC8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AD8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AE8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="AH8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="AI8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="AJ8" s="9">
         <v>42635</v>
@@ -2454,36 +2476,36 @@
       </c>
       <c r="AL8" s="11"/>
       <c r="AM8" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO8" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AS8" s="9">
         <v>42712</v>
       </c>
       <c r="AT8" s="9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" t="s">
         <v>102</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="C9" t="s">
-        <v>104</v>
-      </c>
-      <c r="D9" t="s">
-        <v>105</v>
       </c>
       <c r="E9" s="14">
         <v>60</v>
@@ -2498,7 +2520,7 @@
         <v>0.35583120000000001</v>
       </c>
       <c r="I9" s="28" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J9">
         <v>50</v>
@@ -2540,7 +2562,7 @@
         <v>40</v>
       </c>
       <c r="W9" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X9" s="9">
         <v>42551</v>
@@ -2553,22 +2575,22 @@
       </c>
       <c r="AA9" s="14"/>
       <c r="AB9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="AC9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AD9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AE9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="AH9" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="AI9" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="AJ9" s="9">
         <v>42614</v>
@@ -2578,36 +2600,36 @@
       </c>
       <c r="AL9" s="11"/>
       <c r="AM9" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO9" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AS9" s="9">
         <v>42712</v>
       </c>
       <c r="AT9" s="9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D10" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E10" s="14">
         <v>60</v>
@@ -2622,11 +2644,14 @@
         <v>0.35583120000000001</v>
       </c>
       <c r="I10" s="28" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J10">
         <v>60</v>
       </c>
+      <c r="K10" s="42" t="s">
+        <v>297</v>
+      </c>
       <c r="L10">
         <v>60</v>
       </c>
@@ -2652,7 +2677,7 @@
         <v>300</v>
       </c>
       <c r="W10" s="29" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="Y10" s="9">
         <v>42572</v>
@@ -2661,25 +2686,25 @@
         <v>42594</v>
       </c>
       <c r="AB10" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="AC10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AD10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AE10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="AG10" s="9">
         <v>42536</v>
       </c>
       <c r="AH10" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="AI10" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="AJ10" s="9">
         <v>42615</v>
@@ -2689,36 +2714,36 @@
       </c>
       <c r="AL10" s="11"/>
       <c r="AM10" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO10" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AS10" s="9">
         <v>42704</v>
       </c>
       <c r="AT10" s="9" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" t="s">
         <v>112</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="C11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D11" t="s">
-        <v>115</v>
       </c>
       <c r="E11" s="14">
         <v>100</v>
@@ -2733,7 +2758,7 @@
         <v>0.61776249999999999</v>
       </c>
       <c r="I11" s="28" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J11">
         <v>100</v>
@@ -2772,7 +2797,7 @@
         <v>300</v>
       </c>
       <c r="W11" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X11" s="9">
         <v>42550</v>
@@ -2784,22 +2809,22 @@
         <v>42594</v>
       </c>
       <c r="AB11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC11" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>95</v>
+      </c>
+      <c r="AH11" t="s">
         <v>53</v>
       </c>
-      <c r="AD11" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>98</v>
-      </c>
-      <c r="AH11" t="s">
-        <v>56</v>
-      </c>
       <c r="AI11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="AJ11" s="9">
         <v>42615</v>
@@ -2809,36 +2834,36 @@
       </c>
       <c r="AL11" s="11"/>
       <c r="AM11" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO11" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AS11" s="9">
         <v>42704</v>
       </c>
       <c r="AT11" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" t="s">
+        <v>116</v>
+      </c>
+      <c r="D12" t="s">
         <v>117</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="C12" t="s">
-        <v>119</v>
-      </c>
-      <c r="D12" t="s">
-        <v>120</v>
       </c>
       <c r="E12" s="14">
         <v>50</v>
@@ -2853,7 +2878,7 @@
         <v>0.49420999999999998</v>
       </c>
       <c r="I12" s="28" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J12">
         <v>50</v>
@@ -2895,7 +2920,7 @@
         <v>0</v>
       </c>
       <c r="W12" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X12" s="9">
         <v>42548</v>
@@ -2907,25 +2932,25 @@
         <v>42594</v>
       </c>
       <c r="AB12" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="AC12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AD12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AE12" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="AG12" s="9">
         <v>42625</v>
       </c>
       <c r="AH12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="AI12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="AJ12" s="9">
         <v>42628</v>
@@ -2935,36 +2960,36 @@
       </c>
       <c r="AL12" s="11"/>
       <c r="AM12" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO12" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AS12" s="9">
         <v>42695</v>
       </c>
       <c r="AT12" s="9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C13" t="s">
+        <v>121</v>
+      </c>
+      <c r="D13" t="s">
         <v>122</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="C13" t="s">
-        <v>124</v>
-      </c>
-      <c r="D13" t="s">
-        <v>125</v>
       </c>
       <c r="E13" s="14">
         <v>50</v>
@@ -2979,10 +3004,13 @@
         <v>0.162347985</v>
       </c>
       <c r="I13" s="28" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J13">
         <v>50</v>
+      </c>
+      <c r="K13" s="42" t="s">
+        <v>297</v>
       </c>
       <c r="L13">
         <v>50</v>
@@ -3012,7 +3040,7 @@
         <v>20</v>
       </c>
       <c r="W13" s="29" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="Y13" s="9">
         <v>42571</v>
@@ -3024,22 +3052,22 @@
         <v>42599</v>
       </c>
       <c r="AB13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="AC13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AD13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AE13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="AH13" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="AI13" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="AJ13" s="9">
         <v>42628</v>
@@ -3049,36 +3077,36 @@
       </c>
       <c r="AL13" s="11"/>
       <c r="AM13" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO13" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AS13" s="9">
         <v>42695</v>
       </c>
       <c r="AT13" s="9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C14" t="s">
+        <v>125</v>
+      </c>
+      <c r="D14" t="s">
         <v>126</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="C14" t="s">
-        <v>128</v>
-      </c>
-      <c r="D14" t="s">
-        <v>129</v>
       </c>
       <c r="E14" s="14">
         <v>100</v>
@@ -3093,18 +3121,18 @@
         <v>0.77442707</v>
       </c>
       <c r="I14" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="J14">
-        <v>100</v>
-      </c>
-      <c r="K14">
-        <v>50</v>
-      </c>
-      <c r="L14">
-        <v>50</v>
-      </c>
-      <c r="M14">
+        <v>47</v>
+      </c>
+      <c r="J14" s="43">
+        <v>100</v>
+      </c>
+      <c r="K14" s="43">
+        <v>50</v>
+      </c>
+      <c r="L14" s="43">
+        <v>50</v>
+      </c>
+      <c r="M14" s="43">
         <v>100</v>
       </c>
       <c r="N14">
@@ -3135,7 +3163,7 @@
         <v>160</v>
       </c>
       <c r="W14" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X14" s="9">
         <v>42550</v>
@@ -3148,22 +3176,22 @@
       </c>
       <c r="AA14" s="9"/>
       <c r="AB14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="AC14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AD14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AE14" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="AH14" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="AI14" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="AJ14" s="9">
         <v>42627</v>
@@ -3173,36 +3201,36 @@
       </c>
       <c r="AL14" s="11"/>
       <c r="AM14" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN14" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO14" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP14" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AS14" s="9">
         <v>42711</v>
       </c>
       <c r="AT14" s="9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C15" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D15" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E15" s="14">
         <v>100</v>
@@ -3217,7 +3245,7 @@
         <v>0.49420999999999998</v>
       </c>
       <c r="I15" s="28" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J15">
         <v>100</v>
@@ -3256,7 +3284,7 @@
         <v>30</v>
       </c>
       <c r="W15" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X15" s="9">
         <v>42548</v>
@@ -3271,25 +3299,25 @@
         <v>42599</v>
       </c>
       <c r="AB15" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="AC15" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="AD15" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="AE15" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="AG15" s="9">
         <v>42576</v>
       </c>
       <c r="AH15" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AI15" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AJ15" s="9">
         <v>42624</v>
@@ -3299,36 +3327,36 @@
       </c>
       <c r="AL15" s="11"/>
       <c r="AM15" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO15" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AS15" s="9">
         <v>42705</v>
       </c>
       <c r="AT15" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C16" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D16" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E16" s="14">
         <v>100</v>
@@ -3343,10 +3371,13 @@
         <v>0.49420999999999998</v>
       </c>
       <c r="I16" s="28" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J16">
         <v>100</v>
+      </c>
+      <c r="K16" s="42" t="s">
+        <v>297</v>
       </c>
       <c r="L16">
         <v>100</v>
@@ -3370,7 +3401,7 @@
         <v>10</v>
       </c>
       <c r="W16" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="Y16" s="9">
         <v>42571</v>
@@ -3379,25 +3410,25 @@
         <v>42592</v>
       </c>
       <c r="AB16" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="AC16" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="AD16" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="AE16" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="AG16" s="9">
         <v>42576</v>
       </c>
       <c r="AH16" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AI16" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AJ16" s="9">
         <v>42624</v>
@@ -3407,36 +3438,36 @@
       </c>
       <c r="AL16" s="11"/>
       <c r="AM16" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO16" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AS16" s="9">
         <v>42705</v>
       </c>
       <c r="AT16" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="C17" t="s">
+        <v>138</v>
+      </c>
+      <c r="D17" t="s">
         <v>139</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="C17" t="s">
-        <v>141</v>
-      </c>
-      <c r="D17" t="s">
-        <v>142</v>
       </c>
       <c r="E17" s="28">
         <v>75</v>
@@ -3451,7 +3482,7 @@
         <v>1.1119725</v>
       </c>
       <c r="I17" s="28" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="J17">
         <v>80</v>
@@ -3493,7 +3524,7 @@
         <v>80</v>
       </c>
       <c r="W17" s="30" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="X17" s="9">
         <v>42548</v>
@@ -3505,22 +3536,22 @@
         <v>42594</v>
       </c>
       <c r="AB17" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="AC17" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="AD17" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="AE17" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="AH17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="AI17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="AJ17" s="9">
         <v>42662</v>
@@ -3528,10 +3559,10 @@
       <c r="AK17" s="10"/>
       <c r="AL17" s="11"/>
       <c r="AM17" s="14" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="AN17" s="14" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="AO17" s="12"/>
       <c r="AP17" s="12"/>
@@ -3539,21 +3570,21 @@
         <v>42707</v>
       </c>
       <c r="AT17" s="9" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C18" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D18" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E18" s="28">
         <v>75</v>
@@ -3568,7 +3599,7 @@
         <v>1.1119725</v>
       </c>
       <c r="I18" s="28" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="J18">
         <v>80</v>
@@ -3610,7 +3641,7 @@
         <v>80</v>
       </c>
       <c r="W18" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X18" s="9">
         <v>42548</v>
@@ -3622,22 +3653,22 @@
         <v>42594</v>
       </c>
       <c r="AB18" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="AC18" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AD18" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AE18" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="AH18" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="AI18" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="AJ18" s="9">
         <v>42621</v>
@@ -3647,42 +3678,42 @@
       </c>
       <c r="AL18" s="11"/>
       <c r="AM18" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN18" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO18" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP18" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AS18" s="9">
         <v>42707</v>
       </c>
       <c r="AT18" s="9" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C19" t="s">
+        <v>152</v>
+      </c>
+      <c r="D19" t="s">
         <v>153</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="E19" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="C19" t="s">
+      <c r="F19" s="7" t="s">
         <v>155</v>
-      </c>
-      <c r="D19" t="s">
-        <v>156</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>158</v>
       </c>
       <c r="G19">
         <v>860</v>
@@ -3691,7 +3722,7 @@
         <v>0.21251030000000001</v>
       </c>
       <c r="I19" s="28" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="J19">
         <v>60</v>
@@ -3730,7 +3761,7 @@
         <v>30</v>
       </c>
       <c r="W19" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X19" s="9">
         <v>42550</v>
@@ -3742,25 +3773,25 @@
         <v>42594</v>
       </c>
       <c r="AB19" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="AC19" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AD19" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AE19" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="AG19" s="9">
         <v>42587</v>
       </c>
       <c r="AH19" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AI19" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AJ19" s="9">
         <v>42617</v>
@@ -3770,42 +3801,42 @@
       </c>
       <c r="AL19" s="11"/>
       <c r="AM19" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO19" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AS19" s="9">
         <v>42705</v>
       </c>
       <c r="AT19" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="C20" t="s">
+        <v>159</v>
+      </c>
+      <c r="D20" t="s">
         <v>160</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="E20" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="C20" t="s">
+      <c r="F20" s="7" t="s">
         <v>162</v>
-      </c>
-      <c r="D20" t="s">
-        <v>163</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>165</v>
       </c>
       <c r="G20">
         <v>860</v>
@@ -3814,7 +3845,7 @@
         <v>0.21251030000000001</v>
       </c>
       <c r="I20" s="28" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="J20">
         <v>60</v>
@@ -3853,7 +3884,7 @@
         <v>30</v>
       </c>
       <c r="W20" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X20" s="9">
         <v>42550</v>
@@ -3865,25 +3896,25 @@
         <v>42594</v>
       </c>
       <c r="AB20" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="AC20" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AD20" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AE20" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="AG20" s="9">
         <v>42587</v>
       </c>
       <c r="AH20" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AI20" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AJ20" s="9">
         <v>42617</v>
@@ -3893,36 +3924,36 @@
       </c>
       <c r="AL20" s="11"/>
       <c r="AM20" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN20" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO20" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP20" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AS20" s="9">
         <v>42705</v>
       </c>
       <c r="AT20" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C21" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D21" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E21">
         <v>100</v>
@@ -3937,18 +3968,18 @@
         <v>0.49420999999999998</v>
       </c>
       <c r="I21" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="J21">
-        <v>100</v>
-      </c>
-      <c r="K21">
-        <v>50</v>
-      </c>
-      <c r="L21" s="15">
-        <v>50</v>
-      </c>
-      <c r="M21">
+        <v>93</v>
+      </c>
+      <c r="J21" s="43">
+        <v>100</v>
+      </c>
+      <c r="K21" s="43">
+        <v>50</v>
+      </c>
+      <c r="L21" s="43">
+        <v>50</v>
+      </c>
+      <c r="M21" s="43">
         <v>100</v>
       </c>
       <c r="N21">
@@ -3976,7 +4007,7 @@
         <v>60</v>
       </c>
       <c r="W21" s="29" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="X21" s="9">
         <v>42550</v>
@@ -3988,22 +4019,22 @@
         <v>42594</v>
       </c>
       <c r="AB21" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="AC21" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AD21" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AE21" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="AH21" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="AI21" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="AJ21" s="9">
         <v>42615</v>
@@ -4013,36 +4044,36 @@
       </c>
       <c r="AL21" s="11"/>
       <c r="AM21" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN21" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO21" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP21" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AS21" s="9">
         <v>42704</v>
       </c>
       <c r="AT21" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C22" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D22" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E22">
         <v>100</v>
@@ -4057,18 +4088,18 @@
         <v>0.49420999999999998</v>
       </c>
       <c r="I22" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="J22">
-        <v>100</v>
-      </c>
-      <c r="K22">
-        <v>50</v>
-      </c>
-      <c r="L22" s="15">
-        <v>50</v>
-      </c>
-      <c r="M22">
+        <v>93</v>
+      </c>
+      <c r="J22" s="43">
+        <v>100</v>
+      </c>
+      <c r="K22" s="43">
+        <v>50</v>
+      </c>
+      <c r="L22" s="43">
+        <v>50</v>
+      </c>
+      <c r="M22" s="43">
         <v>100</v>
       </c>
       <c r="N22">
@@ -4096,7 +4127,7 @@
         <v>60</v>
       </c>
       <c r="W22" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X22" s="9">
         <v>42550</v>
@@ -4108,22 +4139,22 @@
         <v>42594</v>
       </c>
       <c r="AB22" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="AC22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AD22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AE22" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="AH22" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="AI22" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="AJ22" s="9">
         <v>42615</v>
@@ -4133,36 +4164,36 @@
       </c>
       <c r="AL22" s="11"/>
       <c r="AM22" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN22" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO22" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP22" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AS22" s="9">
         <v>42704</v>
       </c>
       <c r="AT22" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="C23" t="s">
+        <v>172</v>
+      </c>
+      <c r="D23" t="s">
         <v>173</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="C23" t="s">
-        <v>175</v>
-      </c>
-      <c r="D23" t="s">
-        <v>176</v>
       </c>
       <c r="E23">
         <v>50</v>
@@ -4177,10 +4208,16 @@
         <v>0.18532874999999999</v>
       </c>
       <c r="I23" s="28" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J23">
         <v>50</v>
+      </c>
+      <c r="K23" s="42" t="s">
+        <v>297</v>
+      </c>
+      <c r="L23" s="42" t="s">
+        <v>297</v>
       </c>
       <c r="M23">
         <v>50</v>
@@ -4201,31 +4238,31 @@
         <v>80</v>
       </c>
       <c r="W23" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="Z23" s="9">
         <v>42597</v>
       </c>
       <c r="AB23" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="AC23" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AD23" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AE23" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="AG23" s="9">
         <v>42628</v>
       </c>
       <c r="AH23" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="AI23" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="AJ23" s="9">
         <v>42648</v>
@@ -4235,36 +4272,36 @@
       </c>
       <c r="AL23" s="11"/>
       <c r="AM23" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN23" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO23" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP23" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AS23" s="9">
         <v>42710</v>
       </c>
       <c r="AT23" s="9" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="24" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C24" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="E24" s="15">
         <v>70</v>
@@ -4280,18 +4317,18 @@
         <v>0.51892050000000001</v>
       </c>
       <c r="I24" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="J24">
+        <v>65</v>
+      </c>
+      <c r="J24" s="43">
         <v>70</v>
       </c>
-      <c r="K24">
-        <v>100</v>
-      </c>
-      <c r="L24">
-        <v>100</v>
-      </c>
-      <c r="M24">
+      <c r="K24" s="43">
+        <v>100</v>
+      </c>
+      <c r="L24" s="43">
+        <v>100</v>
+      </c>
+      <c r="M24" s="43">
         <v>100</v>
       </c>
       <c r="N24">
@@ -4322,7 +4359,7 @@
         <v>600</v>
       </c>
       <c r="W24" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X24" s="9">
         <v>42551</v>
@@ -4334,22 +4371,22 @@
         <v>42593</v>
       </c>
       <c r="AB24" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="AC24" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="AD24" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="AE24" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="AH24" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="AI24" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="AJ24" s="12"/>
       <c r="AK24" s="12"/>
@@ -4364,21 +4401,21 @@
         <v>42712</v>
       </c>
       <c r="AT24" s="9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:64" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="C25" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="D25" s="31" t="s">
         <v>185</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="C25" s="31" t="s">
-        <v>187</v>
-      </c>
-      <c r="D25" s="31" t="s">
-        <v>188</v>
       </c>
       <c r="E25" s="31">
         <v>25</v>
@@ -4394,18 +4431,18 @@
         <v>0.13096565000000002</v>
       </c>
       <c r="I25" s="32" t="s">
-        <v>143</v>
-      </c>
-      <c r="J25" s="31">
+        <v>140</v>
+      </c>
+      <c r="J25" s="44">
         <v>30</v>
       </c>
-      <c r="K25" s="31">
-        <v>50</v>
-      </c>
-      <c r="L25" s="31">
-        <v>50</v>
-      </c>
-      <c r="M25" s="31">
+      <c r="K25" s="44">
+        <v>50</v>
+      </c>
+      <c r="L25" s="44">
+        <v>50</v>
+      </c>
+      <c r="M25" s="44">
         <v>30</v>
       </c>
       <c r="N25" s="31">
@@ -4427,7 +4464,7 @@
         <v>20</v>
       </c>
       <c r="W25" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X25" s="33">
         <v>42551</v>
@@ -4440,22 +4477,22 @@
       </c>
       <c r="AA25" s="33"/>
       <c r="AB25" s="31" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="AC25" s="31" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AE25" s="31" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="AG25" s="33">
         <v>42615</v>
       </c>
       <c r="AH25" s="31" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AI25" s="33" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="BA25" s="34"/>
       <c r="BB25" s="34"/>
@@ -4472,16 +4509,16 @@
     </row>
     <row r="26" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C26" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D26" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E26">
         <v>100</v>
@@ -4496,7 +4533,7 @@
         <v>0.49420999999999998</v>
       </c>
       <c r="I26" s="28" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J26">
         <v>100</v>
@@ -4538,7 +4575,7 @@
         <v>20</v>
       </c>
       <c r="W26" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X26" s="9">
         <v>42551</v>
@@ -4550,25 +4587,25 @@
         <v>42593</v>
       </c>
       <c r="AB26" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="AC26" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AD26" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AE26" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="AG26" s="9">
         <v>42612</v>
       </c>
       <c r="AH26" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AI26" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AJ26" s="9">
         <v>42627</v>
@@ -4578,36 +4615,36 @@
       </c>
       <c r="AL26" s="11"/>
       <c r="AM26" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN26" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO26" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP26" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AS26" s="9">
         <v>42712</v>
       </c>
       <c r="AT26" s="9" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="27" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C27" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D27" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E27">
         <v>100</v>
@@ -4622,7 +4659,7 @@
         <v>0.49420999999999998</v>
       </c>
       <c r="I27" s="28" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J27">
         <v>100</v>
@@ -4664,7 +4701,7 @@
         <v>80</v>
       </c>
       <c r="W27" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X27" s="9">
         <v>42551</v>
@@ -4676,25 +4713,25 @@
         <v>42593</v>
       </c>
       <c r="AB27" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="AC27" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AD27" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AE27" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="AG27" s="9">
         <v>42612</v>
       </c>
       <c r="AH27" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AI27" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AJ27" s="9">
         <v>42627</v>
@@ -4704,36 +4741,36 @@
       </c>
       <c r="AL27" s="11"/>
       <c r="AM27" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN27" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO27" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP27" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AS27" s="9">
         <v>42712</v>
       </c>
       <c r="AT27" s="9" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="28" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="D28" s="20" t="s">
         <v>198</v>
-      </c>
-      <c r="B28" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="C28" s="20" t="s">
-        <v>200</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>201</v>
       </c>
       <c r="E28" s="20">
         <v>106</v>
@@ -4748,7 +4785,7 @@
         <v>0.86486750000000001</v>
       </c>
       <c r="I28" s="35" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J28" s="20">
         <v>100</v>
@@ -4788,7 +4825,7 @@
       </c>
       <c r="V28" s="20"/>
       <c r="W28" s="36" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X28" s="24">
         <v>42550</v>
@@ -4801,26 +4838,26 @@
       </c>
       <c r="AA28" s="20"/>
       <c r="AB28" s="20" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="AC28" s="20" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AD28" s="20" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AE28" s="20" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="AF28" s="20"/>
       <c r="AG28" s="24">
         <v>42614</v>
       </c>
       <c r="AH28" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="AI28" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="AJ28" s="24">
         <v>42627</v>
@@ -4830,16 +4867,16 @@
       </c>
       <c r="AL28" s="26"/>
       <c r="AM28" s="19" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN28" s="20" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO28" s="19" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP28" s="20" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AQ28" s="20"/>
       <c r="AR28" s="20"/>
@@ -4847,21 +4884,21 @@
         <v>42711</v>
       </c>
       <c r="AT28" s="24" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="29" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="C29" t="s">
+        <v>203</v>
+      </c>
+      <c r="D29" s="15" t="s">
         <v>204</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>205</v>
-      </c>
-      <c r="C29" t="s">
-        <v>206</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>207</v>
       </c>
       <c r="E29" s="14">
         <v>35</v>
@@ -4876,7 +4913,7 @@
         <v>8.6486750000000001E-2</v>
       </c>
       <c r="I29" s="28" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J29">
         <v>30</v>
@@ -4918,7 +4955,7 @@
         <v>90</v>
       </c>
       <c r="W29" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X29" s="37">
         <v>42548</v>
@@ -4933,22 +4970,22 @@
         <v>42599</v>
       </c>
       <c r="AB29" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="AC29" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AD29" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="AE29" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="AH29" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="AI29" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="AJ29" s="9">
         <v>42662</v>
@@ -4956,10 +4993,10 @@
       <c r="AK29" s="12"/>
       <c r="AL29" s="15"/>
       <c r="AM29" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO29" s="38"/>
       <c r="AP29" s="38"/>
@@ -4969,21 +5006,21 @@
         <v>42713</v>
       </c>
       <c r="AT29" s="17" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="30" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="C30" t="s">
+        <v>209</v>
+      </c>
+      <c r="D30" t="s">
         <v>210</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>211</v>
-      </c>
-      <c r="C30" t="s">
-        <v>212</v>
-      </c>
-      <c r="D30" t="s">
-        <v>213</v>
       </c>
       <c r="E30" s="14">
         <v>54</v>
@@ -4998,7 +5035,7 @@
         <v>0.26687339999999998</v>
       </c>
       <c r="I30" s="28" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J30">
         <v>50</v>
@@ -5040,7 +5077,7 @@
         <v>300</v>
       </c>
       <c r="W30" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X30" s="37">
         <v>42548</v>
@@ -5052,25 +5089,25 @@
         <v>42593</v>
       </c>
       <c r="AB30" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="AC30" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AD30" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AE30" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="AG30" s="9">
         <v>42619</v>
       </c>
       <c r="AH30" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="AI30" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="AJ30" s="9">
         <v>42641</v>
@@ -5082,40 +5119,40 @@
         <v>42662</v>
       </c>
       <c r="AM30" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN30" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO30" s="14" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="AP30" s="14"/>
       <c r="AQ30" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AR30" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AS30" s="9">
         <v>42710</v>
       </c>
       <c r="AT30" s="39" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="31" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="C31" t="s">
+        <v>216</v>
+      </c>
+      <c r="D31" t="s">
         <v>217</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>218</v>
-      </c>
-      <c r="C31" t="s">
-        <v>219</v>
-      </c>
-      <c r="D31" t="s">
-        <v>220</v>
       </c>
       <c r="E31" s="14">
         <v>50</v>
@@ -5130,7 +5167,7 @@
         <v>0.24710499999999999</v>
       </c>
       <c r="I31" s="28" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J31">
         <v>50</v>
@@ -5172,7 +5209,7 @@
         <v>200</v>
       </c>
       <c r="W31" s="30" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="X31" s="37">
         <v>42548</v>
@@ -5184,22 +5221,22 @@
         <v>42593</v>
       </c>
       <c r="AB31" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="AC31" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="AD31" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="AE31" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="AH31" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="AI31" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="AJ31" s="9">
         <v>42662</v>
@@ -5209,36 +5246,36 @@
       </c>
       <c r="AL31" s="11"/>
       <c r="AM31" s="14" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="AN31" s="14" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="AO31" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP31" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AS31" s="17">
         <v>42713</v>
       </c>
       <c r="AT31" s="17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C32" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D32" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E32" s="14">
         <v>50</v>
@@ -5253,7 +5290,7 @@
         <v>0.18532874999999999</v>
       </c>
       <c r="I32" s="28" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="J32">
         <v>50</v>
@@ -5295,7 +5332,7 @@
         <v>380</v>
       </c>
       <c r="W32" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X32" s="37">
         <v>42548</v>
@@ -5310,25 +5347,25 @@
         <v>42599</v>
       </c>
       <c r="AB32" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="AC32" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AD32" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AE32" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="AG32" s="9">
         <v>42614</v>
       </c>
       <c r="AH32" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="AI32" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="AJ32" s="9">
         <v>42622</v>
@@ -5338,36 +5375,36 @@
       </c>
       <c r="AL32" s="11"/>
       <c r="AM32" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN32" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO32" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP32" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AS32" s="17">
         <v>42713</v>
       </c>
       <c r="AT32" s="17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="C33" t="s">
+        <v>225</v>
+      </c>
+      <c r="D33" t="s">
         <v>226</v>
-      </c>
-      <c r="B33" s="14" t="s">
-        <v>227</v>
-      </c>
-      <c r="C33" t="s">
-        <v>228</v>
-      </c>
-      <c r="D33" t="s">
-        <v>229</v>
       </c>
       <c r="E33" s="14">
         <v>50</v>
@@ -5382,7 +5419,7 @@
         <v>0.14826300000000001</v>
       </c>
       <c r="I33" s="28" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J33">
         <v>50</v>
@@ -5424,7 +5461,7 @@
         <v>200</v>
       </c>
       <c r="W33" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X33" s="37">
         <v>42548</v>
@@ -5439,25 +5476,25 @@
         <v>42599</v>
       </c>
       <c r="AB33" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="AC33" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AD33" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AE33" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="AG33" s="9">
         <v>42639</v>
       </c>
       <c r="AH33" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="AI33" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="AJ33" s="11">
         <v>42662</v>
@@ -5467,36 +5504,36 @@
       </c>
       <c r="AL33" s="11"/>
       <c r="AM33" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN33" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO33" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP33" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AS33" s="9">
         <v>42710</v>
       </c>
       <c r="AT33" s="9" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="34" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C34" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D34" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E34" s="14">
         <v>50</v>
@@ -5511,7 +5548,7 @@
         <v>0.14826300000000001</v>
       </c>
       <c r="I34" s="28" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J34">
         <v>50</v>
@@ -5550,7 +5587,7 @@
         <v>350</v>
       </c>
       <c r="W34" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X34" s="37">
         <v>42548</v>
@@ -5565,22 +5602,22 @@
         <v>42599</v>
       </c>
       <c r="AB34" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="AC34" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AD34" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AE34" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="AH34" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="AI34" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="AJ34" s="9">
         <v>42619</v>
@@ -5590,36 +5627,36 @@
       </c>
       <c r="AL34" s="11"/>
       <c r="AM34" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN34" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO34" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP34" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AS34" s="9">
         <v>42710</v>
       </c>
       <c r="AT34" s="9" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="35" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
+        <v>232</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="D35" s="20" t="s">
         <v>235</v>
-      </c>
-      <c r="B35" s="19" t="s">
-        <v>236</v>
-      </c>
-      <c r="C35" s="20" t="s">
-        <v>237</v>
-      </c>
-      <c r="D35" s="20" t="s">
-        <v>238</v>
       </c>
       <c r="E35" s="20">
         <v>50</v>
@@ -5634,7 +5671,7 @@
         <v>0.16061824999999999</v>
       </c>
       <c r="I35" s="22" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J35" s="20">
         <v>50</v>
@@ -5674,7 +5711,7 @@
       </c>
       <c r="V35" s="20"/>
       <c r="W35" s="23" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="X35" s="40">
         <v>42548</v>
@@ -5689,24 +5726,24 @@
         <v>42599</v>
       </c>
       <c r="AB35" s="20" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="AC35" s="20" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="AD35" s="20" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="AE35" s="20" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="AF35" s="20"/>
       <c r="AG35" s="20"/>
       <c r="AH35" s="20" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="AI35" s="20" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="AJ35" s="24">
         <v>42662</v>
@@ -5714,10 +5751,10 @@
       <c r="AK35" s="25"/>
       <c r="AL35" s="26"/>
       <c r="AM35" s="20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN35" s="20" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO35" s="27"/>
       <c r="AP35" s="27"/>
@@ -5727,21 +5764,21 @@
         <v>42710</v>
       </c>
       <c r="AT35" s="24" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="36" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="C36" t="s">
+        <v>241</v>
+      </c>
+      <c r="D36" t="s">
         <v>242</v>
-      </c>
-      <c r="B36" s="14" t="s">
-        <v>243</v>
-      </c>
-      <c r="C36" t="s">
-        <v>244</v>
-      </c>
-      <c r="D36" t="s">
-        <v>245</v>
       </c>
       <c r="E36" s="14">
         <v>83</v>
@@ -5756,18 +5793,18 @@
         <v>0.44231795000000002</v>
       </c>
       <c r="I36" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="J36">
+        <v>47</v>
+      </c>
+      <c r="J36" s="43">
         <v>80</v>
       </c>
-      <c r="K36" s="14">
+      <c r="K36" s="45">
         <v>80</v>
       </c>
-      <c r="L36" s="14">
+      <c r="L36" s="45">
         <v>80</v>
       </c>
-      <c r="M36" s="14">
+      <c r="M36" s="45">
         <v>70</v>
       </c>
       <c r="N36" s="14">
@@ -5795,7 +5832,7 @@
         <v>80</v>
       </c>
       <c r="W36" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X36" s="37">
         <v>42552</v>
@@ -5808,22 +5845,22 @@
       </c>
       <c r="AA36" s="14"/>
       <c r="AB36" s="14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC36" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD36" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE36" t="s">
+        <v>243</v>
+      </c>
+      <c r="AH36" t="s">
         <v>53</v>
       </c>
-      <c r="AD36" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE36" t="s">
-        <v>246</v>
-      </c>
-      <c r="AH36" t="s">
-        <v>56</v>
-      </c>
       <c r="AI36" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="AJ36" s="9">
         <v>42614</v>
@@ -5833,36 +5870,36 @@
       </c>
       <c r="AL36" s="11"/>
       <c r="AM36" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN36" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO36" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP36" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="AS36" s="9">
         <v>42706</v>
       </c>
       <c r="AT36" s="9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="37" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C37" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D37" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E37" s="14">
         <v>100</v>
@@ -5877,7 +5914,7 @@
         <v>0.49420999999999998</v>
       </c>
       <c r="I37" s="28" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J37">
         <v>100</v>
@@ -5916,7 +5953,7 @@
         <v>80</v>
       </c>
       <c r="W37" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X37" s="37">
         <v>42552</v>
@@ -5929,22 +5966,22 @@
       </c>
       <c r="AA37" s="14"/>
       <c r="AB37" s="14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC37" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD37" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE37" t="s">
+        <v>243</v>
+      </c>
+      <c r="AH37" t="s">
         <v>53</v>
       </c>
-      <c r="AD37" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE37" t="s">
-        <v>246</v>
-      </c>
-      <c r="AH37" t="s">
-        <v>56</v>
-      </c>
       <c r="AI37" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="AJ37" s="9">
         <v>42614</v>
@@ -5954,36 +5991,36 @@
       </c>
       <c r="AL37" s="11"/>
       <c r="AM37" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN37" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO37" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP37" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="AS37" s="9">
         <v>42706</v>
       </c>
       <c r="AT37" s="9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="38" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="C38" t="s">
+        <v>251</v>
+      </c>
+      <c r="D38" t="s">
         <v>252</v>
-      </c>
-      <c r="B38" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="C38" t="s">
-        <v>254</v>
-      </c>
-      <c r="D38" t="s">
-        <v>255</v>
       </c>
       <c r="E38" s="14">
         <v>100</v>
@@ -5998,7 +6035,7 @@
         <v>0.29652600000000001</v>
       </c>
       <c r="I38" s="28" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J38">
         <v>100</v>
@@ -6037,7 +6074,7 @@
         <v>80</v>
       </c>
       <c r="W38" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X38" s="37">
         <v>42552</v>
@@ -6050,22 +6087,22 @@
       </c>
       <c r="AA38" s="14"/>
       <c r="AB38" s="14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC38" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD38" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE38" t="s">
+        <v>243</v>
+      </c>
+      <c r="AH38" t="s">
         <v>53</v>
       </c>
-      <c r="AD38" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE38" t="s">
-        <v>246</v>
-      </c>
-      <c r="AH38" t="s">
-        <v>56</v>
-      </c>
       <c r="AI38" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="AJ38" s="9">
         <v>42614</v>
@@ -6075,42 +6112,42 @@
       </c>
       <c r="AL38" s="11"/>
       <c r="AM38" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN38" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO38" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP38" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="AS38" s="9">
         <v>42706</v>
       </c>
       <c r="AT38" s="9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="39" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B39" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="C39" t="s">
+        <v>254</v>
+      </c>
+      <c r="D39" t="s">
+        <v>255</v>
+      </c>
+      <c r="E39" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="C39" t="s">
-        <v>257</v>
-      </c>
-      <c r="D39" t="s">
-        <v>258</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>259</v>
-      </c>
       <c r="F39" s="7" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="G39">
         <v>1900</v>
@@ -6119,7 +6156,7 @@
         <v>0.46949950000000001</v>
       </c>
       <c r="I39" s="28" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="J39">
         <v>50</v>
@@ -6158,7 +6195,7 @@
         <v>80</v>
       </c>
       <c r="W39" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X39" s="37">
         <v>42552</v>
@@ -6170,22 +6207,22 @@
         <v>42594</v>
       </c>
       <c r="AB39" s="14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC39" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD39" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE39" t="s">
+        <v>243</v>
+      </c>
+      <c r="AH39" t="s">
         <v>53</v>
       </c>
-      <c r="AD39" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE39" t="s">
-        <v>246</v>
-      </c>
-      <c r="AH39" t="s">
-        <v>56</v>
-      </c>
       <c r="AI39" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="AJ39" s="9">
         <v>42614</v>
@@ -6195,36 +6232,36 @@
       </c>
       <c r="AL39" s="11"/>
       <c r="AM39" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN39" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO39" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP39" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="AS39" s="9">
         <v>42706</v>
       </c>
       <c r="AT39" s="9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="40" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="C40" t="s">
+        <v>260</v>
+      </c>
+      <c r="D40" t="s">
         <v>261</v>
-      </c>
-      <c r="B40" s="14" t="s">
-        <v>262</v>
-      </c>
-      <c r="C40" t="s">
-        <v>263</v>
-      </c>
-      <c r="D40" t="s">
-        <v>264</v>
       </c>
       <c r="E40" s="7">
         <v>108</v>
@@ -6239,7 +6276,7 @@
         <v>0.64247299999999996</v>
       </c>
       <c r="I40" s="28" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J40">
         <v>100</v>
@@ -6281,7 +6318,7 @@
         <v>80</v>
       </c>
       <c r="W40" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X40" s="37">
         <v>42552</v>
@@ -6294,22 +6331,22 @@
       </c>
       <c r="AA40" s="14"/>
       <c r="AB40" s="14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC40" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD40" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE40" t="s">
+        <v>243</v>
+      </c>
+      <c r="AH40" t="s">
         <v>53</v>
       </c>
-      <c r="AD40" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE40" t="s">
-        <v>246</v>
-      </c>
-      <c r="AH40" t="s">
-        <v>56</v>
-      </c>
       <c r="AI40" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="AJ40" s="9">
         <v>42614</v>
@@ -6319,42 +6356,42 @@
       </c>
       <c r="AL40" s="11"/>
       <c r="AM40" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN40" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO40" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP40" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="AS40" s="9">
         <v>42706</v>
       </c>
       <c r="AT40" s="9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="41" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B41" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="C41" t="s">
+        <v>263</v>
+      </c>
+      <c r="D41" t="s">
+        <v>264</v>
+      </c>
+      <c r="E41" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="C41" t="s">
-        <v>266</v>
-      </c>
-      <c r="D41" t="s">
-        <v>267</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>268</v>
-      </c>
       <c r="F41" s="7" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="G41">
         <v>450</v>
@@ -6363,7 +6400,7 @@
         <v>0.11119725</v>
       </c>
       <c r="I41" s="28" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="J41" s="7">
         <v>50</v>
@@ -6405,7 +6442,7 @@
         <v>80</v>
       </c>
       <c r="W41" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X41" s="37">
         <v>42552</v>
@@ -6417,22 +6454,22 @@
         <v>42594</v>
       </c>
       <c r="AB41" s="14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC41" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD41" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE41" t="s">
+        <v>243</v>
+      </c>
+      <c r="AH41" t="s">
         <v>53</v>
       </c>
-      <c r="AD41" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE41" t="s">
-        <v>246</v>
-      </c>
-      <c r="AH41" t="s">
-        <v>56</v>
-      </c>
       <c r="AI41" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="AJ41" s="9">
         <v>42614</v>
@@ -6442,36 +6479,36 @@
       </c>
       <c r="AL41" s="11"/>
       <c r="AM41" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN41" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO41" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP41" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="AS41" s="9">
         <v>42706</v>
       </c>
       <c r="AT41" s="9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="42" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="C42" t="s">
+        <v>269</v>
+      </c>
+      <c r="D42" t="s">
         <v>270</v>
-      </c>
-      <c r="B42" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="C42" t="s">
-        <v>272</v>
-      </c>
-      <c r="D42" t="s">
-        <v>273</v>
       </c>
       <c r="E42" s="7">
         <v>90</v>
@@ -6486,7 +6523,7 @@
         <v>0.51892050000000001</v>
       </c>
       <c r="I42" s="28" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J42">
         <v>80</v>
@@ -6525,7 +6562,7 @@
         <v>80</v>
       </c>
       <c r="W42" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X42" s="37">
         <v>42552</v>
@@ -6537,22 +6574,22 @@
         <v>42594</v>
       </c>
       <c r="AB42" s="14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC42" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD42" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE42" t="s">
+        <v>243</v>
+      </c>
+      <c r="AH42" t="s">
         <v>53</v>
       </c>
-      <c r="AD42" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE42" t="s">
-        <v>246</v>
-      </c>
-      <c r="AH42" t="s">
-        <v>56</v>
-      </c>
       <c r="AI42" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="AJ42" s="9">
         <v>42614</v>
@@ -6562,36 +6599,36 @@
       </c>
       <c r="AL42" s="11"/>
       <c r="AM42" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN42" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO42" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP42" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="AS42" s="9">
         <v>42706</v>
       </c>
       <c r="AT42" s="9" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="43" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C43" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D43" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E43">
         <v>100</v>
@@ -6606,7 +6643,7 @@
         <v>0.24710499999999999</v>
       </c>
       <c r="I43" s="28" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J43">
         <v>100</v>
@@ -6648,7 +6685,7 @@
         <v>80</v>
       </c>
       <c r="W43" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="X43" s="37">
         <v>42552</v>
@@ -6660,22 +6697,22 @@
         <v>42594</v>
       </c>
       <c r="AB43" s="14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC43" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD43" t="s">
+        <v>274</v>
+      </c>
+      <c r="AE43" t="s">
+        <v>243</v>
+      </c>
+      <c r="AH43" t="s">
         <v>53</v>
       </c>
-      <c r="AD43" t="s">
-        <v>277</v>
-      </c>
-      <c r="AE43" t="s">
-        <v>246</v>
-      </c>
-      <c r="AH43" t="s">
-        <v>56</v>
-      </c>
       <c r="AI43" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="AJ43" s="9">
         <v>42614</v>
@@ -6685,36 +6722,36 @@
       </c>
       <c r="AL43" s="11"/>
       <c r="AM43" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN43" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO43" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP43" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="AS43" s="9">
         <v>42706</v>
       </c>
       <c r="AT43" s="9" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="44" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="C44" t="s">
+        <v>278</v>
+      </c>
+      <c r="D44" t="s">
         <v>279</v>
-      </c>
-      <c r="B44" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="C44" t="s">
-        <v>281</v>
-      </c>
-      <c r="D44" t="s">
-        <v>282</v>
       </c>
       <c r="E44">
         <v>55</v>
@@ -6729,10 +6766,13 @@
         <v>0.20386162499999999</v>
       </c>
       <c r="I44" s="28" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J44">
         <v>50</v>
+      </c>
+      <c r="K44" s="42" t="s">
+        <v>297</v>
       </c>
       <c r="L44">
         <v>50</v>
@@ -6762,7 +6802,7 @@
         <v>20</v>
       </c>
       <c r="W44" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="Y44" s="37">
         <v>42565</v>
@@ -6771,22 +6811,22 @@
         <v>42597</v>
       </c>
       <c r="AB44" s="14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC44" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD44" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE44" t="s">
+        <v>243</v>
+      </c>
+      <c r="AH44" t="s">
         <v>53</v>
       </c>
-      <c r="AD44" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE44" t="s">
-        <v>246</v>
-      </c>
-      <c r="AH44" t="s">
-        <v>56</v>
-      </c>
       <c r="AI44" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="AJ44" s="9">
         <v>42614</v>
@@ -6796,36 +6836,36 @@
       </c>
       <c r="AL44" s="11"/>
       <c r="AM44" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN44" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO44" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP44" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="AS44" s="9">
         <v>42713</v>
       </c>
       <c r="AT44" s="9" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="45" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="C45" t="s">
+        <v>283</v>
+      </c>
+      <c r="D45" t="s">
         <v>284</v>
-      </c>
-      <c r="B45" s="14" t="s">
-        <v>285</v>
-      </c>
-      <c r="C45" t="s">
-        <v>286</v>
-      </c>
-      <c r="D45" t="s">
-        <v>287</v>
       </c>
       <c r="E45">
         <v>55</v>
@@ -6840,10 +6880,13 @@
         <v>6.7953874999999997E-2</v>
       </c>
       <c r="I45" s="28" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J45">
         <v>50</v>
+      </c>
+      <c r="K45" s="42" t="s">
+        <v>297</v>
       </c>
       <c r="L45">
         <v>50</v>
@@ -6873,7 +6916,7 @@
         <v>20</v>
       </c>
       <c r="W45" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="Y45" s="37">
         <v>42565</v>
@@ -6882,22 +6925,22 @@
         <v>42597</v>
       </c>
       <c r="AB45" s="14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC45" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD45" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE45" t="s">
+        <v>243</v>
+      </c>
+      <c r="AH45" t="s">
         <v>53</v>
       </c>
-      <c r="AD45" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE45" t="s">
-        <v>246</v>
-      </c>
-      <c r="AH45" t="s">
-        <v>56</v>
-      </c>
       <c r="AI45" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="AJ45" s="9">
         <v>42614</v>
@@ -6907,36 +6950,36 @@
       </c>
       <c r="AL45" s="11"/>
       <c r="AM45" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN45" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO45" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP45" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="AS45" s="9">
         <v>42713</v>
       </c>
       <c r="AT45" s="9" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="46" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="C46" t="s">
+        <v>287</v>
+      </c>
+      <c r="D46" t="s">
         <v>288</v>
-      </c>
-      <c r="B46" s="14" t="s">
-        <v>289</v>
-      </c>
-      <c r="C46" t="s">
-        <v>290</v>
-      </c>
-      <c r="D46" t="s">
-        <v>291</v>
       </c>
       <c r="E46">
         <v>30</v>
@@ -6951,11 +6994,14 @@
         <v>0.14826300000000001</v>
       </c>
       <c r="I46" s="28" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J46">
         <v>30</v>
       </c>
+      <c r="K46" s="42" t="s">
+        <v>297</v>
+      </c>
       <c r="L46">
         <v>30</v>
       </c>
@@ -6981,7 +7027,7 @@
         <v>80</v>
       </c>
       <c r="W46" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="Y46" s="37">
         <v>42570</v>
@@ -6990,22 +7036,22 @@
         <v>42594</v>
       </c>
       <c r="AB46" s="14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC46" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD46" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE46" t="s">
+        <v>243</v>
+      </c>
+      <c r="AH46" t="s">
         <v>53</v>
       </c>
-      <c r="AD46" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE46" t="s">
-        <v>246</v>
-      </c>
-      <c r="AH46" t="s">
-        <v>56</v>
-      </c>
       <c r="AI46" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="AJ46" s="9">
         <v>42627</v>
@@ -7015,36 +7061,36 @@
       </c>
       <c r="AL46" s="11"/>
       <c r="AM46" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN46" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO46" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP46" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AS46" s="9">
         <v>42705</v>
       </c>
       <c r="AT46" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="C47" t="s">
+        <v>291</v>
+      </c>
+      <c r="D47" t="s">
         <v>292</v>
-      </c>
-      <c r="B47" s="14" t="s">
-        <v>293</v>
-      </c>
-      <c r="C47" t="s">
-        <v>294</v>
-      </c>
-      <c r="D47" t="s">
-        <v>295</v>
       </c>
       <c r="E47">
         <v>54</v>
@@ -7059,11 +7105,17 @@
         <v>0.24710499999999999</v>
       </c>
       <c r="I47" s="28" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J47">
         <v>50</v>
       </c>
+      <c r="K47" s="42" t="s">
+        <v>297</v>
+      </c>
+      <c r="L47" s="42" t="s">
+        <v>297</v>
+      </c>
       <c r="M47">
         <v>50</v>
       </c>
@@ -7083,28 +7135,28 @@
         <v>100</v>
       </c>
       <c r="W47" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="Z47" s="37">
         <v>42597</v>
       </c>
       <c r="AB47" s="14" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="AC47" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AD47" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AE47" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="AH47" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="AI47" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="AJ47" s="9">
         <v>42627</v>
@@ -7114,26 +7166,26 @@
       </c>
       <c r="AL47" s="11"/>
       <c r="AM47" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AN47" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AO47" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP47" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AS47" s="17">
         <v>42713</v>
       </c>
       <c r="AT47" s="17" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>